<commit_message>
in progress aliianz expat
</commit_message>
<xml_diff>
--- a/Input/Allianz_Expat_Protect/benefits.xlsx
+++ b/Input/Allianz_Expat_Protect/benefits.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="95">
   <si>
     <t xml:space="preserve">PlanName</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">copayOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deductible</t>
   </si>
   <si>
     <t xml:space="preserve">Pack Premium</t>
@@ -277,6 +280,9 @@
     <t xml:space="preserve">NIL</t>
   </si>
   <si>
+    <t xml:space="preserve">IP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pack Confort</t>
   </si>
   <si>
@@ -296,6 +302,9 @@
   </si>
   <si>
     <t xml:space="preserve">10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OP</t>
   </si>
   <si>
     <t xml:space="preserve">20%</t>
@@ -309,7 +318,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -331,18 +340,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -387,8 +384,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -402,14 +403,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -429,540 +422,547 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB13"/>
+  <dimension ref="A1:BC13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AP1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AX9" activeCellId="0" sqref="AX9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AW1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BB5" activeCellId="0" sqref="BB5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="21.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="24.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="189.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BB1" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="BC1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="N2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="J3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE2" s="1" t="s">
+      <c r="V3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AF2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH2" s="1" t="s">
+      <c r="X3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AF3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AI3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AK3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AL3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AM3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AO2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AN3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AT2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AX2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AR3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AX3" s="4" t="s">
+      <c r="AO3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="BB3" s="2" t="s">
-        <v>90</v>
+      <c r="BB3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="BC3" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX4" s="4" t="s">
+      <c r="AX4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="BB4" s="2" t="s">
-        <v>91</v>
+      <c r="BB4" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX5" s="4" t="s">
+      <c r="AX5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX6" s="4" t="s">
+      <c r="AX6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX7" s="4" t="s">
+      <c r="AX7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX8" s="4" t="s">
+      <c r="AX8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX9" s="4" t="s">
+      <c r="AX9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX10" s="4" t="s">
+      <c r="AX10" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX11" s="4" t="s">
+      <c r="AX11" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX12" s="5" t="s">
+      <c r="AX12" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AX13" s="5" t="s">
+      <c r="AX13" s="0" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>